<commit_message>
Report is almost done, proofreading is only Todo
</commit_message>
<xml_diff>
--- a/Documentation/Measurements.xlsx
+++ b/Documentation/Measurements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikla\Documents\GitHub\PrYlf-Laser\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C492C938-8352-4318-9AC2-922C20F88AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03FEF46-5B45-4D52-AD61-EF396F14D119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="604nm (2)" sheetId="4" r:id="rId1"/>
@@ -1880,7 +1880,7 @@
                   <c:v>521.3365</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>583.75149999999996</c:v>
+                  <c:v>596.23449999999991</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>639.92499999999995</c:v>
@@ -1913,7 +1913,7 @@
                   <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3.1</c:v>
@@ -2065,7 +2065,7 @@
                   <c:v>521.3365</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>583.75149999999996</c:v>
+                  <c:v>596.23449999999991</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>639.92499999999995</c:v>
@@ -2083,7 +2083,7 @@
                   <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3.1</c:v>
@@ -5396,7 +5396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{461506CA-81C5-4F7A-92EE-89B87F4E237F}">
   <dimension ref="B1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -5537,8 +5537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:F18"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="118" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25"/>
@@ -5585,14 +5585,14 @@
     </row>
     <row r="6" spans="2:6">
       <c r="B6">
-        <v>605</v>
+        <v>615</v>
       </c>
       <c r="C6">
         <f>1.2483*B6-171.47</f>
-        <v>583.75149999999996</v>
+        <v>596.23449999999991</v>
       </c>
       <c r="D6">
-        <v>1.6</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="7" spans="2:6">

</xml_diff>